<commit_message>
Added another person's review
</commit_message>
<xml_diff>
--- a/4630f2020/survey/Mobile App Survey.xlsx
+++ b/4630f2020/survey/Mobile App Survey.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentuml-my.sharepoint.com/personal/allan_mccombs_student_uml_edu/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2E3AFD02-94A6-4D21-9EFB-B901ADC54A4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AC9764AD-39E6-4AA0-8A1E-B7925BDA1823}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34320" yWindow="1260" windowWidth="16620" windowHeight="13635" xr2:uid="{4882C089-5715-4D5F-AB41-2916DF5B2D65}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="51">
   <si>
     <t>Person ID</t>
   </si>
@@ -165,6 +165,27 @@
   </si>
   <si>
     <t>Have the ability to add, or have barcode scanner, own drinks</t>
+  </si>
+  <si>
+    <t>Cam</t>
+  </si>
+  <si>
+    <t>Tracking Macronutrients</t>
+  </si>
+  <si>
+    <t>Carb Manager</t>
+  </si>
+  <si>
+    <t>Tracks carbs, fat, protein. Able to track weight loss over weeks / months. Has a lot of brand names' macros</t>
+  </si>
+  <si>
+    <t>Always asks to get premium when opening app, cant get rid of "Carb" tracker bar</t>
+  </si>
+  <si>
+    <t>Ability to change "Carb" tracker bar into "Protein" tracker bar</t>
+  </si>
+  <si>
+    <t>Electrician</t>
   </si>
 </sst>
 </file>
@@ -516,19 +537,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{143B15E2-61F5-4059-8F6B-9E29845C9404}">
-  <dimension ref="A3:J13"/>
+  <dimension ref="A3:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="86.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="59.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="97.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="73.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="55.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
@@ -713,6 +734,35 @@
         <v>17</v>
       </c>
     </row>
+    <row r="15" spans="1:10">
+      <c r="A15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15">
+        <v>22</v>
+      </c>
+      <c r="H15" t="s">
+        <v>24</v>
+      </c>
+      <c r="I15" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -725,6 +775,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D1C86362D7E504A9CD6EC7C08872847" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0b5e47c490171939337c6ae3d5ecdf01">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="644b8d3d-6a61-4b01-828a-d674e9f6b7fa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a0ea37e3483275f4dd3368c1a7eaa266" ns3:_="">
     <xsd:import namespace="644b8d3d-6a61-4b01-828a-d674e9f6b7fa"/>
@@ -870,23 +929,14 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CA7BBD6-6AE3-42D2-B2BF-A5BC6F186F19}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4EDBB3EE-3E41-471B-BAEE-024378CC4253}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{92B860A4-328E-465F-8A29-558077A620C3}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4EDBB3EE-3E41-471B-BAEE-024378CC4253}"/>
 </file>
</xml_diff>